<commit_message>
Fixes #323 - Batch metadata overlay: Support editing components and sub-components.
</commit_message>
<xml_diff>
--- a/test/resources/xls_batch_edit_input_test.xlsx
+++ b/test/resources/xls_batch_edit_input_test.xlsx
@@ -837,7 +837,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="1021">
   <si>
     <t>Object Unique ID</t>
   </si>
@@ -3892,9 +3892,6 @@
     <t>ARK</t>
   </si>
   <si>
-    <t>http://library.ucsd.edu/ark:/20775/zzxxxxxxxx</t>
-  </si>
-  <si>
     <t>collection(s)</t>
   </si>
   <si>
@@ -3953,6 +3950,24 @@
   </si>
   <si>
     <t>anyValue</t>
+  </si>
+  <si>
+    <t>zzxxxxxxxx/1</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Test Component 1</t>
+  </si>
+  <si>
+    <t>zzxxxxxxxx/2</t>
+  </si>
+  <si>
+    <t>Sub-Component</t>
+  </si>
+  <si>
+    <t>Test Sub-Component 1</t>
   </si>
 </sst>
 </file>
@@ -4140,10 +4155,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4205,11 +4224,15 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 4" xfId="1"/>
@@ -4828,7 +4851,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4836,15 +4859,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AI4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
     <col min="4" max="7" width="22.1640625" customWidth="1"/>
     <col min="8" max="8" width="59.83203125" customWidth="1"/>
     <col min="9" max="10" width="57.33203125" customWidth="1"/>
@@ -4936,10 +4961,10 @@
         <v>982</v>
       </c>
       <c r="V1" s="27" t="s">
+        <v>1010</v>
+      </c>
+      <c r="W1" s="27" t="s">
         <v>1011</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>1012</v>
       </c>
       <c r="X1" s="27" t="s">
         <v>984</v>
@@ -4972,19 +4997,16 @@
         <v>993</v>
       </c>
       <c r="AH1" s="27" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="AI1" s="27" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="2" spans="1:35">
       <c r="A2" s="2" t="s">
         <v>975</v>
       </c>
-      <c r="B2" t="s">
-        <v>995</v>
-      </c>
       <c r="C2" s="2" t="s">
         <v>146</v>
       </c>
@@ -5016,10 +5038,10 @@
         <v>972</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>13</v>
@@ -5028,7 +5050,7 @@
         <v>158</v>
       </c>
       <c r="Q2" s="29" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="R2" t="s">
         <v>979</v>
@@ -5043,46 +5065,68 @@
         <v>983</v>
       </c>
       <c r="V2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="W2" t="s">
         <v>1009</v>
       </c>
-      <c r="W2" t="s">
-        <v>1010</v>
-      </c>
       <c r="X2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="Y2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="Z2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="AA2" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="AB2" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="AC2" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="AD2" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="AE2" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="AF2" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="AG2" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="AH2" s="31" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="AI2" s="31" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35">
+      <c r="A3" t="s">
         <v>1015</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add tests for unit field batch overlay.
</commit_message>
<xml_diff>
--- a/test/resources/xls_batch_edit_input_test.xlsx
+++ b/test/resources/xls_batch_edit_input_test.xlsx
@@ -837,7 +837,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="1025">
   <si>
     <t>Object Unique ID</t>
   </si>
@@ -3968,6 +3968,18 @@
   </si>
   <si>
     <t>Test Sub-Component 1</t>
+  </si>
+  <si>
+    <t>Subject:topic FAST</t>
+  </si>
+  <si>
+    <t>Subject:genre FAST</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -4155,10 +4167,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4224,7 +4237,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -4233,6 +4246,7 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 4" xfId="1"/>
@@ -4851,7 +4865,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4859,10 +4873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI4"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4875,28 +4889,28 @@
     <col min="9" max="10" width="57.33203125" customWidth="1"/>
     <col min="11" max="11" width="29.83203125" customWidth="1"/>
     <col min="12" max="12" width="22.6640625" customWidth="1"/>
-    <col min="15" max="16" width="12.83203125" customWidth="1"/>
-    <col min="17" max="17" width="28.5" customWidth="1"/>
-    <col min="18" max="18" width="17.33203125" customWidth="1"/>
-    <col min="19" max="19" width="15.5" customWidth="1"/>
-    <col min="20" max="20" width="20.33203125" customWidth="1"/>
-    <col min="21" max="21" width="11.6640625" customWidth="1"/>
+    <col min="15" max="18" width="12.83203125" customWidth="1"/>
+    <col min="19" max="19" width="28.5" customWidth="1"/>
+    <col min="20" max="20" width="17.33203125" customWidth="1"/>
+    <col min="21" max="21" width="15.5" customWidth="1"/>
     <col min="22" max="22" width="20.33203125" customWidth="1"/>
-    <col min="23" max="23" width="17.83203125" customWidth="1"/>
-    <col min="24" max="24" width="23.1640625" customWidth="1"/>
-    <col min="25" max="25" width="22.6640625" customWidth="1"/>
-    <col min="26" max="26" width="22.83203125" customWidth="1"/>
-    <col min="27" max="27" width="24.83203125" customWidth="1"/>
-    <col min="28" max="28" width="18.5" customWidth="1"/>
-    <col min="29" max="29" width="18.6640625" customWidth="1"/>
-    <col min="30" max="30" width="14.6640625" customWidth="1"/>
-    <col min="31" max="31" width="15" customWidth="1"/>
-    <col min="32" max="32" width="15.6640625" customWidth="1"/>
-    <col min="33" max="33" width="16.83203125" customWidth="1"/>
-    <col min="34" max="34" width="16.6640625" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
+    <col min="24" max="24" width="20.33203125" customWidth="1"/>
+    <col min="25" max="25" width="17.83203125" customWidth="1"/>
+    <col min="26" max="26" width="23.1640625" customWidth="1"/>
+    <col min="27" max="27" width="22.6640625" customWidth="1"/>
+    <col min="28" max="28" width="22.83203125" customWidth="1"/>
+    <col min="29" max="29" width="24.83203125" customWidth="1"/>
+    <col min="30" max="30" width="18.5" customWidth="1"/>
+    <col min="31" max="31" width="18.6640625" customWidth="1"/>
+    <col min="32" max="32" width="14.6640625" customWidth="1"/>
+    <col min="33" max="33" width="15" customWidth="1"/>
+    <col min="34" max="34" width="15.6640625" customWidth="1"/>
+    <col min="35" max="35" width="16.83203125" customWidth="1"/>
+    <col min="36" max="36" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="28">
+    <row r="1" spans="1:38" ht="28">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -4942,68 +4956,77 @@
       <c r="O1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P1" s="28" t="s">
+        <v>1021</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>1022</v>
+      </c>
+      <c r="R1" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="S1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="T1" s="27" t="s">
         <v>976</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="U1" s="27" t="s">
         <v>977</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="V1" s="27" t="s">
         <v>980</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="W1" s="27" t="s">
         <v>982</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="X1" s="27" t="s">
         <v>1010</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="Y1" s="27" t="s">
         <v>1011</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="Z1" s="27" t="s">
         <v>984</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="AA1" s="27" t="s">
         <v>985</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="AB1" s="27" t="s">
         <v>986</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AC1" s="27" t="s">
         <v>987</v>
       </c>
-      <c r="AB1" s="27" t="s">
+      <c r="AD1" s="27" t="s">
         <v>988</v>
       </c>
-      <c r="AC1" s="27" t="s">
+      <c r="AE1" s="27" t="s">
         <v>989</v>
       </c>
-      <c r="AD1" s="27" t="s">
+      <c r="AF1" s="27" t="s">
         <v>990</v>
       </c>
-      <c r="AE1" s="27" t="s">
+      <c r="AG1" s="27" t="s">
         <v>991</v>
       </c>
-      <c r="AF1" s="27" t="s">
+      <c r="AH1" s="27" t="s">
         <v>992</v>
       </c>
-      <c r="AG1" s="27" t="s">
+      <c r="AI1" s="27" t="s">
         <v>993</v>
       </c>
-      <c r="AH1" s="27" t="s">
+      <c r="AJ1" s="27" t="s">
         <v>995</v>
       </c>
-      <c r="AI1" s="27" t="s">
+      <c r="AK1" s="27" t="s">
         <v>1013</v>
       </c>
-    </row>
-    <row r="2" spans="1:35">
+      <c r="AL1" s="27" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
       <c r="A2" s="2" t="s">
         <v>975</v>
       </c>
@@ -5046,68 +5069,77 @@
       <c r="O2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="P2" s="5" t="s">
+        <v>1021</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>1022</v>
+      </c>
+      <c r="R2" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="S2" s="29" t="s">
         <v>996</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>979</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>978</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>981</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>983</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>1008</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>1009</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>1007</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>1006</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>1005</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>1004</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>1003</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>1002</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>1001</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>1000</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>999</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>998</v>
       </c>
-      <c r="AH2" s="31" t="s">
+      <c r="AJ2" s="31" t="s">
         <v>997</v>
       </c>
-      <c r="AI2" s="31" t="s">
+      <c r="AK2" s="31" t="s">
         <v>1014</v>
       </c>
-    </row>
-    <row r="3" spans="1:35">
+      <c r="AL2" s="31" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38">
       <c r="A3" t="s">
         <v>1015</v>
       </c>
@@ -5118,7 +5150,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:38">
       <c r="A4" t="s">
         <v>1018</v>
       </c>

</xml_diff>